<commit_message>
Refactor semantic annotation notebook, add modules
</commit_message>
<xml_diff>
--- a/code/outputs/P1_summary_table.xlsx
+++ b/code/outputs/P1_summary_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,96 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>§ 275.0-2_P1|llm_response</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G5" t="n">
+        <v>65</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>documents-2024-11-01-1.json</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>§ 275.0-5_P1|llm_response</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>15</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>documents-2024-11-01-1.json</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>§ 275.0-7_P1|llm_response</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>19</v>
+      </c>
+      <c r="G7" t="n">
+        <v>36</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>documents-2024-11-01-1.json</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>